<commit_message>
Scikit MLP Classifier Imple
</commit_message>
<xml_diff>
--- a/References/Citations.xlsx
+++ b/References/Citations.xlsx
@@ -3,17 +3,17 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20402"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BD4F1307-7971-4A6F-BA86-AD372C279350}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{61540BE2-31F9-4D62-960C-D70613A91D31}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="9300" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="11160" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Bib" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet1" sheetId="3" r:id="rId2"/>
+    <sheet name="Desc_Table" sheetId="3" r:id="rId2"/>
     <sheet name="Links" sheetId="2" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Bib!$F$1:$F$48</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Bib!$F$1:$F$47</definedName>
   </definedNames>
   <calcPr calcId="162913"/>
   <extLst>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="258" uniqueCount="104">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="258" uniqueCount="105">
   <si>
     <t>Sr. No.</t>
   </si>
@@ -1024,6 +1024,32 @@
   </si>
   <si>
     <t>21-81</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Kaggle, </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Diabetes Prediction(EDA+Classification Algo)</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>, Viewed 21 September 2023,  &lt;https://www.kaggle.com/code/kathanvakharia/diabetes-prediction-eda-classification-algo&gt;</t>
+    </r>
   </si>
 </sst>
 </file>
@@ -1119,7 +1145,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="15">
+  <borders count="6">
     <border>
       <left/>
       <right/>
@@ -1167,159 +1193,20 @@
       <diagonal/>
     </border>
     <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
+      <left/>
+      <right/>
       <top style="thin">
         <color indexed="64"/>
       </top>
-      <bottom style="thin">
+      <bottom style="double">
         <color indexed="64"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
+      <left/>
+      <right/>
       <top/>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
       <bottom style="medium">
         <color indexed="64"/>
       </bottom>
@@ -1330,7 +1217,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="51">
+  <cellXfs count="44">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1409,60 +1296,39 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="5" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="6" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="9" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1743,12 +1609,33 @@
 </a:theme>
 </file>
 
+<file path=xl/webextensions/taskpanes.xml><?xml version="1.0" encoding="utf-8"?>
+<wetp:taskpanes xmlns:wetp="http://schemas.microsoft.com/office/webextensions/taskpanes/2010/11">
+  <wetp:taskpane dockstate="right" visibility="0" width="350" row="4">
+    <wetp:webextensionref xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+  </wetp:taskpane>
+</wetp:taskpanes>
+</file>
+
+<file path=xl/webextensions/webextension1.xml><?xml version="1.0" encoding="utf-8"?>
+<we:webextension xmlns:we="http://schemas.microsoft.com/office/webextensions/webextension/2010/11" id="{2AF65665-8259-45EB-A915-E4212E42F8A6}">
+  <we:reference id="db18cc72-1a17-45df-b60e-7ffb655e8af5" version="1.0.0.4" store="EXCatalog" storeType="EXCatalog"/>
+  <we:alternateReferences>
+    <we:reference id="WA104381701" version="1.0.0.4" store="en-AU" storeType="OMEX"/>
+  </we:alternateReferences>
+  <we:properties/>
+  <we:bindings/>
+  <we:snapshot xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships"/>
+</we:webextension>
+</file>
+
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H48"/>
+  <sheetPr filterMode="1"/>
+  <dimension ref="A1:H47"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="J5" sqref="J5"/>
+    <sheetView tabSelected="1" topLeftCell="A3" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="D18" sqref="D18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1783,7 +1670,7 @@
       <c r="G1" s="19"/>
       <c r="H1" s="31"/>
     </row>
-    <row r="2" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" ht="45" hidden="1" x14ac:dyDescent="0.25">
       <c r="A2" s="3">
         <v>1</v>
       </c>
@@ -1824,7 +1711,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="4" spans="1:8" ht="60" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" ht="60" hidden="1" x14ac:dyDescent="0.25">
       <c r="A4" s="3">
         <v>3</v>
       </c>
@@ -1844,7 +1731,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="5" spans="1:8" ht="60" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" ht="60" hidden="1" x14ac:dyDescent="0.25">
       <c r="A5" s="3">
         <v>4</v>
       </c>
@@ -1912,7 +1799,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="8" spans="1:8" ht="60" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8" ht="60" hidden="1" x14ac:dyDescent="0.25">
       <c r="A8" s="3">
         <v>7</v>
       </c>
@@ -1981,7 +1868,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="11" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:8" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A11" s="3">
         <v>10</v>
       </c>
@@ -2024,7 +1911,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="13" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:8" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A13" s="3">
         <v>12</v>
       </c>
@@ -2064,7 +1951,7 @@
       </c>
       <c r="G14" s="27"/>
     </row>
-    <row r="15" spans="1:8" ht="60" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:8" ht="60" hidden="1" x14ac:dyDescent="0.25">
       <c r="A15" s="3">
         <v>14</v>
       </c>
@@ -2084,7 +1971,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="16" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:8" ht="45" hidden="1" x14ac:dyDescent="0.25">
       <c r="A16" s="3">
         <v>15</v>
       </c>
@@ -2104,7 +1991,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="17" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:8" ht="45" hidden="1" x14ac:dyDescent="0.25">
       <c r="A17" s="3">
         <v>16</v>
       </c>
@@ -2169,7 +2056,7 @@
       </c>
       <c r="G19" s="27"/>
     </row>
-    <row r="20" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:8" ht="45" hidden="1" x14ac:dyDescent="0.25">
       <c r="A20" s="3">
         <v>19</v>
       </c>
@@ -2211,7 +2098,7 @@
       </c>
       <c r="G21" s="27"/>
     </row>
-    <row r="22" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:8" ht="45" hidden="1" x14ac:dyDescent="0.25">
       <c r="A22" s="3">
         <v>21</v>
       </c>
@@ -2231,7 +2118,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="23" spans="1:8" ht="60" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:8" ht="60" hidden="1" x14ac:dyDescent="0.25">
       <c r="A23" s="3">
         <v>22</v>
       </c>
@@ -2251,7 +2138,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="24" spans="1:8" ht="60" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:8" ht="60" hidden="1" x14ac:dyDescent="0.25">
       <c r="A24" s="3">
         <v>23</v>
       </c>
@@ -2271,7 +2158,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="25" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:8" ht="45" hidden="1" x14ac:dyDescent="0.25">
       <c r="A25" s="3">
         <v>24</v>
       </c>
@@ -2291,7 +2178,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="26" spans="1:8" ht="60" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:8" ht="60" hidden="1" x14ac:dyDescent="0.25">
       <c r="A26" s="3">
         <v>25</v>
       </c>
@@ -2313,7 +2200,7 @@
       <c r="G26" s="19"/>
       <c r="H26" s="19"/>
     </row>
-    <row r="27" spans="1:8" ht="75" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:8" ht="75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A27" s="3">
         <v>26</v>
       </c>
@@ -2335,7 +2222,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="28" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:8" ht="45" hidden="1" x14ac:dyDescent="0.25">
       <c r="A28" s="3">
         <v>27</v>
       </c>
@@ -2355,7 +2242,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="29" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:8" ht="45" hidden="1" x14ac:dyDescent="0.25">
       <c r="A29" s="3">
         <v>28</v>
       </c>
@@ -2375,7 +2262,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="30" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:8" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A30" s="3">
         <v>29</v>
       </c>
@@ -2395,7 +2282,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="31" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:8" ht="45" hidden="1" x14ac:dyDescent="0.25">
       <c r="A31" s="3">
         <v>30</v>
       </c>
@@ -2416,7 +2303,7 @@
       </c>
       <c r="G31" s="25"/>
     </row>
-    <row r="32" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:8" ht="45" hidden="1" x14ac:dyDescent="0.25">
       <c r="A32" s="3">
         <v>31</v>
       </c>
@@ -2437,7 +2324,7 @@
       </c>
       <c r="G32" s="31"/>
     </row>
-    <row r="33" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:6" ht="45" hidden="1" x14ac:dyDescent="0.25">
       <c r="A33" s="3">
         <v>32</v>
       </c>
@@ -2457,7 +2344,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="34" spans="1:6" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:6" ht="30.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A34" s="3">
         <v>33</v>
       </c>
@@ -2477,7 +2364,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A35" s="3"/>
       <c r="B35" s="18" t="s">
         <v>66</v>
@@ -2491,21 +2378,25 @@
       </c>
       <c r="F35" s="3"/>
     </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:6" ht="45" hidden="1" x14ac:dyDescent="0.25">
       <c r="A36" s="3"/>
-      <c r="B36" s="18"/>
-      <c r="C36" s="12"/>
+      <c r="B36" s="4" t="s">
+        <v>104</v>
+      </c>
+      <c r="C36" s="9" t="s">
+        <v>9</v>
+      </c>
       <c r="D36" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="E36" s="3" t="s">
+      <c r="E36" s="7" t="s">
         <v>2</v>
       </c>
       <c r="F36" s="3"/>
     </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A37" s="3"/>
-      <c r="B37" s="12"/>
+      <c r="B37" s="18"/>
       <c r="C37" s="12"/>
       <c r="D37" s="3" t="s">
         <v>6</v>
@@ -2515,9 +2406,9 @@
       </c>
       <c r="F37" s="3"/>
     </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A38" s="3"/>
-      <c r="B38" s="18"/>
+      <c r="B38" s="12"/>
       <c r="C38" s="12"/>
       <c r="D38" s="3" t="s">
         <v>6</v>
@@ -2527,9 +2418,9 @@
       </c>
       <c r="F38" s="3"/>
     </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A39" s="3"/>
-      <c r="B39" s="12"/>
+      <c r="B39" s="18"/>
       <c r="C39" s="12"/>
       <c r="D39" s="3" t="s">
         <v>6</v>
@@ -2539,9 +2430,9 @@
       </c>
       <c r="F39" s="3"/>
     </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A40" s="3"/>
-      <c r="B40" s="18"/>
+      <c r="B40" s="12"/>
       <c r="C40" s="12"/>
       <c r="D40" s="3" t="s">
         <v>6</v>
@@ -2551,9 +2442,9 @@
       </c>
       <c r="F40" s="3"/>
     </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A41" s="3"/>
-      <c r="B41" s="12"/>
+      <c r="B41" s="18"/>
       <c r="C41" s="12"/>
       <c r="D41" s="3" t="s">
         <v>6</v>
@@ -2563,9 +2454,9 @@
       </c>
       <c r="F41" s="3"/>
     </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A42" s="3"/>
-      <c r="B42" s="18"/>
+      <c r="B42" s="12"/>
       <c r="C42" s="12"/>
       <c r="D42" s="3" t="s">
         <v>6</v>
@@ -2575,9 +2466,9 @@
       </c>
       <c r="F42" s="3"/>
     </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A43" s="3"/>
-      <c r="B43" s="12"/>
+      <c r="B43" s="18"/>
       <c r="C43" s="12"/>
       <c r="D43" s="3" t="s">
         <v>6</v>
@@ -2587,9 +2478,9 @@
       </c>
       <c r="F43" s="3"/>
     </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A44" s="3"/>
-      <c r="B44" s="18"/>
+      <c r="B44" s="12"/>
       <c r="C44" s="12"/>
       <c r="D44" s="3" t="s">
         <v>6</v>
@@ -2599,9 +2490,9 @@
       </c>
       <c r="F44" s="3"/>
     </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A45" s="3"/>
-      <c r="B45" s="12"/>
+      <c r="B45" s="18"/>
       <c r="C45" s="12"/>
       <c r="D45" s="3" t="s">
         <v>6</v>
@@ -2611,9 +2502,9 @@
       </c>
       <c r="F45" s="3"/>
     </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A46" s="3"/>
-      <c r="B46" s="18"/>
+      <c r="B46" s="12"/>
       <c r="C46" s="12"/>
       <c r="D46" s="3" t="s">
         <v>6</v>
@@ -2623,9 +2514,9 @@
       </c>
       <c r="F46" s="3"/>
     </row>
-    <row r="47" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A47" s="3"/>
-      <c r="B47" s="12"/>
+      <c r="B47" s="18"/>
       <c r="C47" s="12"/>
       <c r="D47" s="3" t="s">
         <v>6</v>
@@ -2635,21 +2526,15 @@
       </c>
       <c r="F47" s="3"/>
     </row>
-    <row r="48" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A48" s="3"/>
-      <c r="B48" s="18"/>
-      <c r="C48" s="12"/>
-      <c r="D48" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="E48" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="F48" s="3"/>
-    </row>
   </sheetData>
-  <autoFilter ref="F1:F48" xr:uid="{85050CBB-4EF8-456A-8648-8583A266FB4B}"/>
-  <sortState ref="A2:H48">
+  <autoFilter ref="F1:F47" xr:uid="{85050CBB-4EF8-456A-8648-8583A266FB4B}">
+    <filterColumn colId="0">
+      <filters>
+        <filter val="Similar Project"/>
+      </filters>
+    </filterColumn>
+  </autoFilter>
+  <sortState ref="A2:H47">
     <sortCondition ref="B11"/>
   </sortState>
   <hyperlinks>
@@ -2721,9 +2606,10 @@
     <hyperlink ref="E13" r:id="rId66" xr:uid="{BA058841-70A9-4578-BDA8-2B610D7F798E}"/>
     <hyperlink ref="D13" r:id="rId67" xr:uid="{E7A0EF1E-D431-4572-B9D4-313436BB39A8}"/>
     <hyperlink ref="B35" r:id="rId68" xr:uid="{4DC081F9-1317-4051-8005-51563B13459B}"/>
+    <hyperlink ref="E36" r:id="rId69" xr:uid="{B110DB8E-16E9-47DF-90DB-9713B248B748}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId69"/>
+  <pageSetup orientation="portrait" r:id="rId70"/>
 </worksheet>
 </file>
 
@@ -2731,15 +2617,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8B9EF1AC-EA86-4B49-9EFB-49A6DAA966B6}">
   <dimension ref="A1:F10"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F10" sqref="A1:F10"/>
+    <sheetView topLeftCell="A2" workbookViewId="0">
+      <selection sqref="A1:F10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="25.5" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="7.28515625" style="1" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="26.85546875" style="1" customWidth="1"/>
-    <col min="3" max="3" width="38.7109375" style="33" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="39.28515625" style="32" customWidth="1"/>
     <col min="4" max="4" width="9.85546875" style="1" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="14" style="1" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="10.85546875" style="1" bestFit="1" customWidth="1"/>
@@ -2747,179 +2633,179 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="47" t="s">
+      <c r="A1" s="34" t="s">
         <v>67</v>
       </c>
-      <c r="B1" s="48" t="s">
+      <c r="B1" s="35" t="s">
         <v>69</v>
       </c>
-      <c r="C1" s="49" t="s">
+      <c r="C1" s="43" t="s">
         <v>70</v>
       </c>
-      <c r="D1" s="49" t="s">
+      <c r="D1" s="34" t="s">
         <v>71</v>
       </c>
-      <c r="E1" s="49" t="s">
+      <c r="E1" s="34" t="s">
         <v>72</v>
       </c>
-      <c r="F1" s="50" t="s">
+      <c r="F1" s="34" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="43">
+    <row r="2" spans="1:6" ht="24" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="36">
         <v>1</v>
       </c>
-      <c r="B2" s="44" t="s">
+      <c r="B2" s="37" t="s">
         <v>74</v>
       </c>
-      <c r="C2" s="45" t="s">
+      <c r="C2" s="38" t="s">
         <v>87</v>
       </c>
-      <c r="D2" s="44" t="s">
+      <c r="D2" s="37" t="s">
         <v>96</v>
       </c>
-      <c r="E2" s="44" t="s">
+      <c r="E2" s="37" t="s">
         <v>82</v>
       </c>
-      <c r="F2" s="46" t="s">
+      <c r="F2" s="37" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="3" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A3" s="38">
-        <v>2</v>
-      </c>
-      <c r="B3" s="3" t="s">
+    <row r="3" spans="1:6" ht="42" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="37">
+        <v>2</v>
+      </c>
+      <c r="B3" s="37" t="s">
         <v>75</v>
       </c>
-      <c r="C3" s="35" t="s">
+      <c r="C3" s="39" t="s">
         <v>88</v>
       </c>
-      <c r="D3" s="3" t="s">
+      <c r="D3" s="37" t="s">
         <v>97</v>
       </c>
-      <c r="E3" s="3" t="s">
+      <c r="E3" s="37" t="s">
         <v>82</v>
       </c>
       <c r="F3" s="37" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="4" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="36">
         <v>3</v>
       </c>
-      <c r="B4" s="3" t="s">
+      <c r="B4" s="37" t="s">
         <v>76</v>
       </c>
-      <c r="C4" s="35" t="s">
+      <c r="C4" s="39" t="s">
         <v>90</v>
       </c>
-      <c r="D4" s="3" t="s">
+      <c r="D4" s="37" t="s">
         <v>98</v>
       </c>
-      <c r="E4" s="3" t="s">
+      <c r="E4" s="37" t="s">
         <v>82</v>
       </c>
       <c r="F4" s="37" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="5" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A5" s="38">
+    <row r="5" spans="1:6" ht="36" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="37">
         <v>4</v>
       </c>
-      <c r="B5" s="3" t="s">
+      <c r="B5" s="37" t="s">
         <v>77</v>
       </c>
-      <c r="C5" s="35" t="s">
+      <c r="C5" s="39" t="s">
         <v>91</v>
       </c>
-      <c r="D5" s="3" t="s">
+      <c r="D5" s="37" t="s">
         <v>99</v>
       </c>
-      <c r="E5" s="3" t="s">
+      <c r="E5" s="37" t="s">
         <v>82</v>
       </c>
       <c r="F5" s="37" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="6" spans="1:6" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="36">
         <v>5</v>
       </c>
-      <c r="B6" s="3" t="s">
+      <c r="B6" s="37" t="s">
         <v>78</v>
       </c>
-      <c r="C6" s="35" t="s">
+      <c r="C6" s="39" t="s">
         <v>89</v>
       </c>
-      <c r="D6" s="3" t="s">
+      <c r="D6" s="37" t="s">
         <v>100</v>
       </c>
-      <c r="E6" s="3" t="s">
+      <c r="E6" s="37" t="s">
         <v>82</v>
       </c>
       <c r="F6" s="37" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="7" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A7" s="38">
-        <v>6</v>
-      </c>
-      <c r="B7" s="3" t="s">
+    <row r="7" spans="1:6" ht="40.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="37">
+        <v>6</v>
+      </c>
+      <c r="B7" s="37" t="s">
         <v>79</v>
       </c>
-      <c r="C7" s="35" t="s">
+      <c r="C7" s="39" t="s">
         <v>92</v>
       </c>
-      <c r="D7" s="3" t="s">
+      <c r="D7" s="37" t="s">
         <v>101</v>
       </c>
-      <c r="E7" s="3" t="s">
+      <c r="E7" s="37" t="s">
         <v>82</v>
       </c>
       <c r="F7" s="37" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="8" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" ht="68.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="36">
         <v>7</v>
       </c>
-      <c r="B8" s="3" t="s">
+      <c r="B8" s="37" t="s">
         <v>86</v>
       </c>
-      <c r="C8" s="35" t="s">
+      <c r="C8" s="39" t="s">
         <v>93</v>
       </c>
-      <c r="D8" s="3" t="s">
+      <c r="D8" s="37" t="s">
         <v>102</v>
       </c>
-      <c r="E8" s="3" t="s">
+      <c r="E8" s="37" t="s">
         <v>82</v>
       </c>
       <c r="F8" s="37" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="9" spans="1:6" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="38">
+    <row r="9" spans="1:6" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="37">
         <v>8</v>
       </c>
-      <c r="B9" s="3" t="s">
+      <c r="B9" s="37" t="s">
         <v>80</v>
       </c>
-      <c r="C9" s="34" t="s">
+      <c r="C9" s="38" t="s">
         <v>94</v>
       </c>
-      <c r="D9" s="3" t="s">
+      <c r="D9" s="37" t="s">
         <v>103</v>
       </c>
-      <c r="E9" s="3" t="s">
+      <c r="E9" s="37" t="s">
         <v>82</v>
       </c>
       <c r="F9" s="37" t="s">
@@ -2927,22 +2813,22 @@
       </c>
     </row>
     <row r="10" spans="1:6" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="39">
+      <c r="A10" s="40">
         <v>9</v>
       </c>
-      <c r="B10" s="40" t="s">
+      <c r="B10" s="41" t="s">
         <v>81</v>
       </c>
-      <c r="C10" s="41" t="s">
+      <c r="C10" s="42" t="s">
         <v>95</v>
       </c>
-      <c r="D10" s="40" t="s">
+      <c r="D10" s="41" t="s">
         <v>68</v>
       </c>
-      <c r="E10" s="40" t="s">
+      <c r="E10" s="41" t="s">
         <v>83</v>
       </c>
-      <c r="F10" s="42" t="s">
+      <c r="F10" s="41" t="s">
         <v>85</v>
       </c>
     </row>
@@ -2963,15 +2849,15 @@
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B1" s="32" t="s">
+      <c r="B1" s="33" t="s">
         <v>53</v>
       </c>
-      <c r="C1" s="32"/>
-      <c r="D1" s="32"/>
-      <c r="E1" s="32"/>
-      <c r="F1" s="32"/>
-      <c r="G1" s="32"/>
-      <c r="H1" s="32"/>
+      <c r="C1" s="33"/>
+      <c r="D1" s="33"/>
+      <c r="E1" s="33"/>
+      <c r="F1" s="33"/>
+      <c r="G1" s="33"/>
+      <c r="H1" s="33"/>
     </row>
     <row r="2" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B2" t="s">

</xml_diff>

<commit_message>
SGD and Adam completed Alpha
</commit_message>
<xml_diff>
--- a/References/Citations.xlsx
+++ b/References/Citations.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20402"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2B895317-A428-49D7-ADC0-C81327125E51}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F5090E4F-96F4-4CDA-AED5-C53D978B95AC}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="17670" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="18600" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Bib" sheetId="1" r:id="rId1"/>
@@ -13,7 +13,7 @@
     <sheet name="Links" sheetId="2" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Bib!$H$2:$H$48</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Bib!$H$1:$H$48</definedName>
   </definedNames>
   <calcPr calcId="162913"/>
   <extLst>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="321" uniqueCount="132">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="319" uniqueCount="131">
   <si>
     <t>Sr. No.</t>
   </si>
@@ -563,9 +563,6 @@
   </si>
   <si>
     <t>Normalization for Preprocessing I guess</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SLP </t>
   </si>
   <si>
     <t>Regression, but probably can be used for extra knowledge anout SLP algo</t>
@@ -1511,7 +1508,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="64">
+  <cellXfs count="66">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1667,12 +1664,16 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1975,10 +1976,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <sheetPr filterMode="1"/>
   <dimension ref="A1:J48"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A14" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="B44" sqref="B44"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="H58" sqref="H58"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2005,7 +2007,7 @@
         <v>15</v>
       </c>
       <c r="D1" s="46" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="E1" s="2" t="s">
         <v>5</v>
@@ -2014,7 +2016,7 @@
         <v>2</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="H1" s="2" t="s">
         <v>3</v>
@@ -2039,13 +2041,13 @@
         <v>2</v>
       </c>
       <c r="G2" s="45" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="H2" s="9" t="s">
+        <v>103</v>
+      </c>
+      <c r="I2" s="41" t="s">
         <v>104</v>
-      </c>
-      <c r="I2" s="41" t="s">
-        <v>105</v>
       </c>
       <c r="J2" s="24"/>
     </row>
@@ -2069,14 +2071,14 @@
         <v>2</v>
       </c>
       <c r="G3" s="45" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="H3" s="3" t="s">
         <v>36</v>
       </c>
       <c r="J3" s="24"/>
     </row>
-    <row r="4" spans="1:10" ht="60" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:10" ht="60" hidden="1" x14ac:dyDescent="0.25">
       <c r="A4" s="3">
         <v>3</v>
       </c>
@@ -2094,14 +2096,14 @@
         <v>2</v>
       </c>
       <c r="G4" s="50" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="H4" s="3" t="s">
         <v>31</v>
       </c>
       <c r="J4" s="12"/>
     </row>
-    <row r="5" spans="1:10" ht="46.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:10" ht="46.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="3">
         <v>4</v>
       </c>
@@ -2117,7 +2119,7 @@
         <v>25</v>
       </c>
       <c r="G5" s="50" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="H5" s="11" t="s">
         <v>24</v>
@@ -2126,12 +2128,12 @@
         <v>27</v>
       </c>
     </row>
-    <row r="6" spans="1:10" ht="60" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:10" ht="60" hidden="1" x14ac:dyDescent="0.25">
       <c r="A6" s="3">
         <v>5</v>
       </c>
       <c r="B6" s="44" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="C6" s="8" t="s">
         <v>8</v>
@@ -2146,7 +2148,7 @@
         <v>2</v>
       </c>
       <c r="G6" s="3" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="H6" s="3"/>
       <c r="J6" s="12"/>
@@ -2156,7 +2158,7 @@
         <v>6</v>
       </c>
       <c r="B7" s="18" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C7" s="9" t="s">
         <v>9</v>
@@ -2171,24 +2173,24 @@
         <v>2</v>
       </c>
       <c r="G7" s="45" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="H7" s="3" t="s">
         <v>36</v>
       </c>
       <c r="I7" s="1" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="J7" s="22" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="8" spans="1:10" ht="45" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:10" ht="45" hidden="1" x14ac:dyDescent="0.25">
       <c r="A8" s="3">
         <v>7</v>
       </c>
       <c r="B8" s="18" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="C8" s="5" t="s">
         <v>7</v>
@@ -2225,18 +2227,18 @@
         <v>2</v>
       </c>
       <c r="G9" s="53" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="H9" s="3" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="10" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:10" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A10" s="3">
         <v>9</v>
       </c>
       <c r="B10" s="18" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="C10" s="5" t="s">
         <v>7</v>
@@ -2254,14 +2256,14 @@
       <c r="H10" s="3"/>
       <c r="J10" s="54"/>
     </row>
-    <row r="11" spans="1:10" s="37" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:10" s="37" customFormat="1" ht="45" hidden="1" x14ac:dyDescent="0.25">
       <c r="A11" s="3">
         <v>10</v>
       </c>
-      <c r="B11" s="62" t="s">
-        <v>127</v>
-      </c>
-      <c r="C11" s="63" t="s">
+      <c r="B11" s="61" t="s">
+        <v>126</v>
+      </c>
+      <c r="C11" s="62" t="s">
         <v>8</v>
       </c>
       <c r="D11" s="48"/>
@@ -2276,12 +2278,12 @@
       <c r="I11" s="1"/>
       <c r="J11" s="55"/>
     </row>
-    <row r="12" spans="1:10" ht="60" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:10" ht="60" hidden="1" x14ac:dyDescent="0.25">
       <c r="A12" s="3">
         <v>11</v>
       </c>
       <c r="B12" s="57" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C12" s="60" t="s">
         <v>9</v>
@@ -2294,7 +2296,7 @@
         <v>2</v>
       </c>
       <c r="G12" s="7" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="H12" s="14" t="s">
         <v>31</v>
@@ -2306,7 +2308,7 @@
         <v>12</v>
       </c>
       <c r="B13" s="4" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C13" s="5" t="s">
         <v>7</v>
@@ -2321,13 +2323,13 @@
         <v>2</v>
       </c>
       <c r="G13" s="45" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="H13" s="3" t="s">
         <v>36</v>
       </c>
       <c r="I13" s="38" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="J13" s="56"/>
     </row>
@@ -2336,7 +2338,7 @@
         <v>13</v>
       </c>
       <c r="B14" s="18" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C14" s="5" t="s">
         <v>7</v>
@@ -2349,24 +2351,24 @@
         <v>2</v>
       </c>
       <c r="G14" s="45" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="H14" s="3" t="s">
         <v>36</v>
       </c>
       <c r="I14" s="38" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="J14" s="20" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="15" spans="1:10" ht="60" x14ac:dyDescent="0.25">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" ht="60" hidden="1" x14ac:dyDescent="0.25">
       <c r="A15" s="3">
         <v>14</v>
       </c>
       <c r="B15" s="23" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C15" s="5" t="s">
         <v>7</v>
@@ -2379,7 +2381,7 @@
         <v>2</v>
       </c>
       <c r="G15" s="11" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="H15" s="3"/>
     </row>
@@ -2403,7 +2405,7 @@
         <v>2</v>
       </c>
       <c r="G16" s="53" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="H16" s="3" t="s">
         <v>37</v>
@@ -2414,7 +2416,7 @@
         <v>16</v>
       </c>
       <c r="B17" s="17" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C17" s="5" t="s">
         <v>7</v>
@@ -2431,15 +2433,15 @@
         <v>36</v>
       </c>
       <c r="I17" s="38" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="18" spans="1:10" ht="45" x14ac:dyDescent="0.25">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10" ht="45" hidden="1" x14ac:dyDescent="0.25">
       <c r="A18" s="3">
         <v>17</v>
       </c>
       <c r="B18" s="4" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="C18" s="9" t="s">
         <v>9</v>
@@ -2454,17 +2456,17 @@
         <v>2</v>
       </c>
       <c r="G18" s="51" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="H18" s="3"/>
       <c r="J18" s="16"/>
     </row>
-    <row r="19" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:10" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A19" s="3">
         <v>18</v>
       </c>
       <c r="B19" s="23" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C19" s="8" t="s">
         <v>8</v>
@@ -2479,7 +2481,7 @@
         <v>2</v>
       </c>
       <c r="G19" s="51" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="H19" s="3"/>
       <c r="J19" s="26"/>
@@ -2502,19 +2504,19 @@
         <v>2</v>
       </c>
       <c r="G20" s="50" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="H20" s="3" t="s">
         <v>36</v>
       </c>
       <c r="I20" s="38"/>
     </row>
-    <row r="21" spans="1:10" ht="60" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:10" ht="60" hidden="1" x14ac:dyDescent="0.25">
       <c r="A21" s="3">
         <v>20</v>
       </c>
       <c r="B21" s="17" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C21" s="5" t="s">
         <v>7</v>
@@ -2530,7 +2532,7 @@
       </c>
       <c r="G21" s="7"/>
       <c r="H21" s="3" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="J21" s="54"/>
     </row>
@@ -2539,7 +2541,7 @@
         <v>21</v>
       </c>
       <c r="B22" s="4" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C22" s="5" t="s">
         <v>7</v>
@@ -2552,13 +2554,11 @@
         <v>2</v>
       </c>
       <c r="G22" s="50" t="s">
-        <v>114</v>
-      </c>
-      <c r="H22" s="3" t="s">
-        <v>38</v>
-      </c>
+        <v>113</v>
+      </c>
+      <c r="H22" s="65"/>
       <c r="I22" s="1" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="J22" s="55"/>
     </row>
@@ -2567,7 +2567,7 @@
         <v>22</v>
       </c>
       <c r="B23" s="18" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="C23" s="5" t="s">
         <v>7</v>
@@ -2580,13 +2580,11 @@
         <v>2</v>
       </c>
       <c r="G23" s="50" t="s">
-        <v>124</v>
-      </c>
-      <c r="H23" s="3" t="s">
-        <v>38</v>
-      </c>
+        <v>123</v>
+      </c>
+      <c r="H23" s="65"/>
       <c r="I23" s="1" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="J23" s="55"/>
     </row>
@@ -2610,7 +2608,7 @@
         <v>2</v>
       </c>
       <c r="G24" s="53" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="H24" s="3" t="s">
         <v>37</v>
@@ -2622,7 +2620,7 @@
         <v>24</v>
       </c>
       <c r="B25" s="18" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C25" s="5" t="s">
         <v>7</v>
@@ -2648,7 +2646,7 @@
         <v>25</v>
       </c>
       <c r="B26" s="17" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C26" s="5" t="s">
         <v>7</v>
@@ -2668,30 +2666,30 @@
       </c>
       <c r="I26" s="38"/>
     </row>
-    <row r="27" spans="1:10" ht="45" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:10" ht="45" hidden="1" x14ac:dyDescent="0.25">
       <c r="A27" s="3">
         <v>26</v>
       </c>
       <c r="B27" s="44" t="s">
+        <v>109</v>
+      </c>
+      <c r="C27" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="D27" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="E27" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="F27" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="G27" s="6" t="s">
+        <v>124</v>
+      </c>
+      <c r="H27" s="3" t="s">
         <v>110</v>
-      </c>
-      <c r="C27" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="D27" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="E27" s="7" t="s">
-        <v>6</v>
-      </c>
-      <c r="F27" s="7" t="s">
-        <v>2</v>
-      </c>
-      <c r="G27" s="6" t="s">
-        <v>125</v>
-      </c>
-      <c r="H27" s="3" t="s">
-        <v>111</v>
       </c>
       <c r="J27" s="16"/>
     </row>
@@ -2713,7 +2711,7 @@
         <v>2</v>
       </c>
       <c r="G28" s="53" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="H28" s="14" t="s">
         <v>37</v>
@@ -2725,7 +2723,7 @@
         <v>28</v>
       </c>
       <c r="B29" s="4" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C29" s="9" t="s">
         <v>9</v>
@@ -2765,14 +2763,14 @@
         <v>2</v>
       </c>
       <c r="G30" s="10" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="H30" s="3" t="s">
         <v>38</v>
       </c>
       <c r="J30" s="37"/>
     </row>
-    <row r="31" spans="1:10" ht="60" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:10" ht="60" hidden="1" x14ac:dyDescent="0.25">
       <c r="A31" s="3">
         <v>30</v>
       </c>
@@ -2790,14 +2788,14 @@
         <v>2</v>
       </c>
       <c r="G31" s="53" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="H31" s="11" t="s">
         <v>12</v>
       </c>
       <c r="J31" s="54"/>
     </row>
-    <row r="32" spans="1:10" ht="60" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:10" ht="60" hidden="1" x14ac:dyDescent="0.25">
       <c r="A32" s="3">
         <v>31</v>
       </c>
@@ -2815,7 +2813,7 @@
         <v>2</v>
       </c>
       <c r="G32" s="50" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="H32" s="3" t="s">
         <v>39</v>
@@ -2823,7 +2821,7 @@
       <c r="I32" s="59"/>
       <c r="J32" s="55"/>
     </row>
-    <row r="33" spans="1:10" ht="45" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:10" ht="45" hidden="1" x14ac:dyDescent="0.25">
       <c r="A33" s="3">
         <v>32</v>
       </c>
@@ -2847,12 +2845,12 @@
       <c r="I33" s="40"/>
       <c r="J33" s="55"/>
     </row>
-    <row r="34" spans="1:10" ht="60" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:10" ht="60" hidden="1" x14ac:dyDescent="0.25">
       <c r="A34" s="3">
         <v>33</v>
       </c>
       <c r="B34" s="4" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C34" s="8" t="s">
         <v>8</v>
@@ -2866,17 +2864,17 @@
       </c>
       <c r="G34" s="7"/>
       <c r="H34" s="3" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="I34" s="40"/>
       <c r="J34" s="56"/>
     </row>
-    <row r="35" spans="1:10" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:10" ht="30.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A35" s="3">
         <v>34</v>
       </c>
       <c r="B35" s="4" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C35" s="8" t="s">
         <v>8</v>
@@ -2892,15 +2890,15 @@
       <c r="H35" s="3"/>
       <c r="I35" s="58"/>
       <c r="J35" s="21" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="36" spans="1:10" ht="45" x14ac:dyDescent="0.25">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="36" spans="1:10" ht="45" hidden="1" x14ac:dyDescent="0.25">
       <c r="A36" s="3">
         <v>35</v>
       </c>
       <c r="B36" s="4" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C36" s="9" t="s">
         <v>9</v>
@@ -2914,7 +2912,7 @@
       </c>
       <c r="G36" s="7"/>
       <c r="H36" s="3" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="I36" s="40"/>
     </row>
@@ -2929,7 +2927,7 @@
         <v>7</v>
       </c>
       <c r="D37" s="9"/>
-      <c r="E37" s="7" t="s">
+      <c r="E37" s="64" t="s">
         <v>6</v>
       </c>
       <c r="F37" s="7" t="s">
@@ -2951,25 +2949,25 @@
       <c r="C38" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="D38" s="47"/>
+      <c r="D38" s="9"/>
       <c r="E38" s="7" t="s">
         <v>6</v>
       </c>
       <c r="F38" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="G38" s="7"/>
-      <c r="H38" s="3" t="s">
-        <v>37</v>
-      </c>
+      <c r="G38" s="50" t="s">
+        <v>113</v>
+      </c>
+      <c r="H38" s="65"/>
       <c r="I38" s="1"/>
     </row>
-    <row r="39" spans="1:10" ht="45" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:10" ht="45" hidden="1" x14ac:dyDescent="0.25">
       <c r="A39" s="3">
         <v>38</v>
       </c>
       <c r="B39" s="4" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C39" s="8" t="s">
         <v>8</v>
@@ -2985,11 +2983,11 @@
       </c>
       <c r="G39" s="7"/>
       <c r="H39" s="3" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="I39" s="40"/>
     </row>
-    <row r="40" spans="1:10" ht="45" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:10" ht="45" hidden="1" x14ac:dyDescent="0.25">
       <c r="A40" s="3">
         <v>39</v>
       </c>
@@ -3022,19 +3020,19 @@
       <c r="C41" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="D41" s="47"/>
+      <c r="D41" s="9"/>
       <c r="E41" s="7" t="s">
         <v>6</v>
       </c>
       <c r="F41" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="G41" s="7"/>
-      <c r="H41" s="3" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="42" spans="1:10" ht="60" x14ac:dyDescent="0.25">
+      <c r="G41" s="50" t="s">
+        <v>113</v>
+      </c>
+      <c r="H41" s="65"/>
+    </row>
+    <row r="42" spans="1:10" ht="60" hidden="1" x14ac:dyDescent="0.25">
       <c r="A42" s="3">
         <v>41</v>
       </c>
@@ -3053,10 +3051,10 @@
       </c>
       <c r="G42" s="7"/>
       <c r="H42" s="11" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="43" spans="1:10" x14ac:dyDescent="0.25">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="43" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A43" s="3"/>
       <c r="B43" s="42"/>
       <c r="C43" s="12"/>
@@ -3070,7 +3068,7 @@
       <c r="G43" s="3"/>
       <c r="H43" s="3"/>
     </row>
-    <row r="44" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A44" s="3"/>
       <c r="B44" s="43"/>
       <c r="C44" s="12"/>
@@ -3084,7 +3082,7 @@
       <c r="G44" s="3"/>
       <c r="H44" s="3"/>
     </row>
-    <row r="45" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A45" s="3"/>
       <c r="B45" s="42"/>
       <c r="C45" s="12"/>
@@ -3098,7 +3096,7 @@
       <c r="G45" s="3"/>
       <c r="H45" s="3"/>
     </row>
-    <row r="46" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A46" s="3"/>
       <c r="B46" s="43"/>
       <c r="C46" s="12"/>
@@ -3112,7 +3110,7 @@
       <c r="G46" s="3"/>
       <c r="H46" s="3"/>
     </row>
-    <row r="47" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A47" s="3"/>
       <c r="B47" s="42"/>
       <c r="C47" s="12"/>
@@ -3126,7 +3124,7 @@
       <c r="G47" s="3"/>
       <c r="H47" s="3"/>
     </row>
-    <row r="48" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A48" s="3"/>
       <c r="B48" s="43"/>
       <c r="C48" s="12"/>
@@ -3141,7 +3139,17 @@
       <c r="H48" s="3"/>
     </row>
   </sheetData>
-  <autoFilter ref="H2:H48" xr:uid="{56DA2A05-69A3-4F93-B5DE-207C7FE39AEF}"/>
+  <autoFilter ref="H1:H48" xr:uid="{CC9D2202-DEE7-40E4-92B9-A5FAB8141FD4}">
+    <filterColumn colId="0">
+      <filters>
+        <filter val="Similar Project"/>
+        <filter val="SLP"/>
+        <filter val="The OG"/>
+        <filter val="Use Case of SLP"/>
+        <filter val="Use Case of SLP_x000a_"/>
+      </filters>
+    </filterColumn>
+  </autoFilter>
   <sortState ref="A2:J48">
     <sortCondition ref="B23"/>
   </sortState>
@@ -3151,82 +3159,82 @@
     <hyperlink ref="E41" r:id="rId3" xr:uid="{C1FFB862-1C41-45BE-A38C-EC798D435A03}"/>
     <hyperlink ref="F41" r:id="rId4" xr:uid="{A781D5BC-5847-489D-811E-6880A507B07B}"/>
     <hyperlink ref="F37" r:id="rId5" xr:uid="{58391554-A585-43A7-8673-D7ABA0FAE245}"/>
-    <hyperlink ref="E37" r:id="rId6" xr:uid="{5FBE1348-598D-4B23-BF70-CD1A45069B6F}"/>
-    <hyperlink ref="E40" r:id="rId7" xr:uid="{04CBC333-821B-44F5-94F2-E77F367D9DCC}"/>
-    <hyperlink ref="F40" r:id="rId8" xr:uid="{E28BBD5D-E04C-456A-9BFB-78D1C6C33BBD}"/>
-    <hyperlink ref="F31" r:id="rId9" xr:uid="{4A664B0A-D6F8-49C7-8C92-DA9C74143276}"/>
-    <hyperlink ref="E31" r:id="rId10" xr:uid="{153BF790-6A77-4F43-8998-AEFF0825A828}"/>
-    <hyperlink ref="F2" r:id="rId11" xr:uid="{1514AAB9-BD28-4F4F-8723-E449E949F916}"/>
-    <hyperlink ref="E2" r:id="rId12" xr:uid="{382E074D-3104-472A-80C7-7B0C3B55A917}"/>
-    <hyperlink ref="E30" r:id="rId13" xr:uid="{75C4EE83-F42C-4DDB-BCC0-B0E1EC7620CA}"/>
-    <hyperlink ref="F30" r:id="rId14" xr:uid="{43F9FD49-0099-43EE-A156-9A658A337A2E}"/>
-    <hyperlink ref="E33" r:id="rId15" xr:uid="{DD765DC4-BF46-4056-8C6E-646ACCA69266}"/>
-    <hyperlink ref="F33" r:id="rId16" xr:uid="{1756CF05-531F-4B7A-B4C9-BECE5F79F8E1}"/>
-    <hyperlink ref="E38" r:id="rId17" xr:uid="{2AB4D467-774B-410E-9786-1B3036659AD0}"/>
-    <hyperlink ref="F38" r:id="rId18" xr:uid="{9DC437E2-9294-47A2-BC5D-A151DF6FF776}"/>
-    <hyperlink ref="F9" r:id="rId19" xr:uid="{2D09C1BD-FC48-4CB4-853A-226D12689519}"/>
-    <hyperlink ref="E42" r:id="rId20" xr:uid="{5CEA8427-8E58-4278-9068-735F05BA9701}"/>
-    <hyperlink ref="F42" r:id="rId21" xr:uid="{AA330F24-940B-43A9-B648-E8AEACC4E9EC}"/>
-    <hyperlink ref="F5" r:id="rId22" xr:uid="{68DB759D-76EA-4874-9304-2BD355C2CC53}"/>
-    <hyperlink ref="J7" r:id="rId23" xr:uid="{87D1748D-BF5D-4A14-AFAE-E37533C3A0D8}"/>
-    <hyperlink ref="E28" r:id="rId24" xr:uid="{934EAA82-CF78-4A74-9CD0-3EDDB2F3D25A}"/>
-    <hyperlink ref="F28" r:id="rId25" xr:uid="{77732C7E-A884-4FCF-BF0E-97717B117A16}"/>
-    <hyperlink ref="E16" r:id="rId26" xr:uid="{E8C37E71-EFD5-47E0-BC97-25AB0FD10F1C}"/>
-    <hyperlink ref="F16" r:id="rId27" xr:uid="{ABE4519E-2F61-44CC-9622-75D9DA5F7D97}"/>
-    <hyperlink ref="E4" r:id="rId28" xr:uid="{31541EE7-B42D-423E-9AA8-C216DE6B64A7}"/>
-    <hyperlink ref="F4" r:id="rId29" xr:uid="{395A83D0-9F08-4D83-854F-0AE6F1F29CBC}"/>
-    <hyperlink ref="F3" r:id="rId30" xr:uid="{58F9AB1E-5488-40A2-9983-26F11E828595}"/>
-    <hyperlink ref="E3" r:id="rId31" xr:uid="{5A8C1A72-92CF-4171-B7B9-E0254CBDE43F}"/>
-    <hyperlink ref="E24" r:id="rId32" xr:uid="{1F2E3E11-4862-43A4-AE5B-A25971038030}"/>
-    <hyperlink ref="F24" r:id="rId33" xr:uid="{82182BB5-27E4-45A0-9245-90B695825443}"/>
-    <hyperlink ref="E9" r:id="rId34" xr:uid="{06ECC9D7-A685-4D13-AE11-5DD9C258A7EE}"/>
-    <hyperlink ref="J5" r:id="rId35" xr:uid="{BEC89C47-1D25-4DE9-AC71-083FAD0B34C3}"/>
-    <hyperlink ref="E20" r:id="rId36" xr:uid="{3FA1CD4F-2381-4BF1-8F3E-F2B2EC7ACF85}"/>
-    <hyperlink ref="E32" r:id="rId37" xr:uid="{6143B28D-A231-422C-9F6E-9D22A5EE20EC}"/>
-    <hyperlink ref="F34" r:id="rId38" xr:uid="{F50C1EB9-5D1C-4B95-B429-377D59A03513}"/>
-    <hyperlink ref="E34" r:id="rId39" xr:uid="{215E8F44-72B5-4AED-B8B7-3F716C2C9FED}"/>
-    <hyperlink ref="E22" r:id="rId40" xr:uid="{00990BE2-D559-46EF-86D1-57D51622C40D}"/>
-    <hyperlink ref="F22" r:id="rId41" xr:uid="{DCD02053-CEBB-4E57-904F-A030DF9C21A9}"/>
-    <hyperlink ref="E12" r:id="rId42" xr:uid="{AEC3391B-7D1E-4D91-B2D0-7C05910F189D}"/>
-    <hyperlink ref="F12" r:id="rId43" xr:uid="{DFC08211-F9CC-4B7C-BE88-90F525577256}"/>
-    <hyperlink ref="F21" r:id="rId44" xr:uid="{DA238934-A9D6-41DF-A7D3-02C52609E7A4}"/>
-    <hyperlink ref="E21" r:id="rId45" xr:uid="{BE1025E4-0C8B-464A-94DB-E1029F52499B}"/>
-    <hyperlink ref="F39" r:id="rId46" xr:uid="{A667CFB0-7B94-472E-9628-6E081DEF139A}"/>
-    <hyperlink ref="E39" r:id="rId47" xr:uid="{1C4AFCD6-DEF8-42D4-A41B-2335EDE91552}"/>
-    <hyperlink ref="F36" r:id="rId48" xr:uid="{6A71B6A8-01BB-4EC2-A1E1-3A9FC5E427FC}"/>
-    <hyperlink ref="E36" r:id="rId49" xr:uid="{A60CB216-EF26-4335-B9A8-9667A0871FCE}"/>
-    <hyperlink ref="F13" r:id="rId50" xr:uid="{BF2B90AA-CB55-4147-84AC-0500086745BF}"/>
-    <hyperlink ref="E13" r:id="rId51" xr:uid="{5A9C1536-19AB-4B66-A33C-E94FAEA8DC33}"/>
-    <hyperlink ref="E26" r:id="rId52" xr:uid="{6B3F056B-BE9E-410D-A402-D0B7A082F8FF}"/>
-    <hyperlink ref="F26" r:id="rId53" xr:uid="{5FFF6BB5-6911-47ED-A878-31F14AA4CCB6}"/>
-    <hyperlink ref="F7" r:id="rId54" xr:uid="{9567CA2D-EFE1-41F8-948A-768765025D60}"/>
-    <hyperlink ref="E7" r:id="rId55" xr:uid="{A1309773-A5F2-461B-9FD5-6F306A4FD457}"/>
-    <hyperlink ref="E29" r:id="rId56" xr:uid="{A162F40D-F6FD-4099-A350-D0002A3057DA}"/>
-    <hyperlink ref="F29" r:id="rId57" xr:uid="{E01788B1-A80B-48E9-9E16-744B2433ED75}"/>
-    <hyperlink ref="F25" r:id="rId58" xr:uid="{779B7301-2CC3-4C4F-8FC3-C6FD68C1B77A}"/>
-    <hyperlink ref="E25" r:id="rId59" xr:uid="{AFCDF617-1F40-451D-88A8-8E755B3BE1D2}"/>
-    <hyperlink ref="E35" r:id="rId60" xr:uid="{FC1DB418-6772-4F8C-82D8-5AF5628D3AC3}"/>
-    <hyperlink ref="F14" r:id="rId61" xr:uid="{16C94B7E-E6C6-4CF0-B928-AD2B73500472}"/>
-    <hyperlink ref="F35" r:id="rId62" location="citeas" xr:uid="{D1B3B81C-2F82-4629-9FC1-4353AB605B76}"/>
-    <hyperlink ref="E14" r:id="rId63" xr:uid="{656876C3-5D28-4ECE-B160-137885BBD472}"/>
-    <hyperlink ref="F17" r:id="rId64" xr:uid="{1CDD0BF3-93DF-4629-8D83-4C995F3FBAEA}"/>
-    <hyperlink ref="E17" r:id="rId65" xr:uid="{1E99DCCD-93C8-47BD-AB1B-F096AD30B672}"/>
-    <hyperlink ref="F19" r:id="rId66" xr:uid="{BA058841-70A9-4578-BDA8-2B610D7F798E}"/>
-    <hyperlink ref="E19" r:id="rId67" xr:uid="{E7A0EF1E-D431-4572-B9D4-313436BB39A8}"/>
-    <hyperlink ref="F18" r:id="rId68" xr:uid="{B110DB8E-16E9-47DF-90DB-9713B248B748}"/>
-    <hyperlink ref="F23" r:id="rId69" xr:uid="{BE0E25E4-720D-43DC-BA86-AC4CAAF9C963}"/>
-    <hyperlink ref="E23" r:id="rId70" xr:uid="{8B9D759F-81A0-4BAB-A68F-F8FAA98330AE}"/>
-    <hyperlink ref="F27" r:id="rId71" xr:uid="{BD2F2414-265C-4ECF-9E09-71CC6602CB5C}"/>
-    <hyperlink ref="E27" r:id="rId72" xr:uid="{FCD02C76-FDEC-49EE-80EF-34CED8D9D6B6}"/>
-    <hyperlink ref="E15" r:id="rId73" xr:uid="{584D0A85-BBC0-4358-BB54-87D73785496D}"/>
-    <hyperlink ref="F11" r:id="rId74" xr:uid="{27264864-EE95-448C-811F-BA85099EF2D9}"/>
-    <hyperlink ref="E11" r:id="rId75" xr:uid="{EEF03948-E49B-486E-817D-EEE788F4CEAE}"/>
-    <hyperlink ref="F10" r:id="rId76" xr:uid="{DE92A6AE-A2E4-46C7-8FFF-C5F1A12E2ACB}"/>
-    <hyperlink ref="E10" r:id="rId77" xr:uid="{F96F71DF-0664-4DD1-88E4-CBDF6565534B}"/>
-    <hyperlink ref="F6" r:id="rId78" xr:uid="{86D7A23D-5E99-4CD5-B311-DD9D8A173C8C}"/>
-    <hyperlink ref="E6" r:id="rId79" xr:uid="{30A4C8C1-66D0-4C23-8217-B4C3DB83F2EA}"/>
-    <hyperlink ref="F8" r:id="rId80" xr:uid="{E4965881-1403-4F79-8959-22D0A974E759}"/>
-    <hyperlink ref="E8" r:id="rId81" xr:uid="{1ACDBBF2-07D0-4487-B5C6-AC33BDA7AF67}"/>
+    <hyperlink ref="E40" r:id="rId6" xr:uid="{04CBC333-821B-44F5-94F2-E77F367D9DCC}"/>
+    <hyperlink ref="F40" r:id="rId7" xr:uid="{E28BBD5D-E04C-456A-9BFB-78D1C6C33BBD}"/>
+    <hyperlink ref="F31" r:id="rId8" xr:uid="{4A664B0A-D6F8-49C7-8C92-DA9C74143276}"/>
+    <hyperlink ref="E31" r:id="rId9" xr:uid="{153BF790-6A77-4F43-8998-AEFF0825A828}"/>
+    <hyperlink ref="F2" r:id="rId10" xr:uid="{1514AAB9-BD28-4F4F-8723-E449E949F916}"/>
+    <hyperlink ref="E2" r:id="rId11" xr:uid="{382E074D-3104-472A-80C7-7B0C3B55A917}"/>
+    <hyperlink ref="E30" r:id="rId12" xr:uid="{75C4EE83-F42C-4DDB-BCC0-B0E1EC7620CA}"/>
+    <hyperlink ref="F30" r:id="rId13" xr:uid="{43F9FD49-0099-43EE-A156-9A658A337A2E}"/>
+    <hyperlink ref="E33" r:id="rId14" xr:uid="{DD765DC4-BF46-4056-8C6E-646ACCA69266}"/>
+    <hyperlink ref="F33" r:id="rId15" xr:uid="{1756CF05-531F-4B7A-B4C9-BECE5F79F8E1}"/>
+    <hyperlink ref="F9" r:id="rId16" xr:uid="{2D09C1BD-FC48-4CB4-853A-226D12689519}"/>
+    <hyperlink ref="E42" r:id="rId17" xr:uid="{5CEA8427-8E58-4278-9068-735F05BA9701}"/>
+    <hyperlink ref="F42" r:id="rId18" xr:uid="{AA330F24-940B-43A9-B648-E8AEACC4E9EC}"/>
+    <hyperlink ref="F5" r:id="rId19" xr:uid="{68DB759D-76EA-4874-9304-2BD355C2CC53}"/>
+    <hyperlink ref="J7" r:id="rId20" xr:uid="{87D1748D-BF5D-4A14-AFAE-E37533C3A0D8}"/>
+    <hyperlink ref="E28" r:id="rId21" xr:uid="{934EAA82-CF78-4A74-9CD0-3EDDB2F3D25A}"/>
+    <hyperlink ref="F28" r:id="rId22" xr:uid="{77732C7E-A884-4FCF-BF0E-97717B117A16}"/>
+    <hyperlink ref="E16" r:id="rId23" xr:uid="{E8C37E71-EFD5-47E0-BC97-25AB0FD10F1C}"/>
+    <hyperlink ref="F16" r:id="rId24" xr:uid="{ABE4519E-2F61-44CC-9622-75D9DA5F7D97}"/>
+    <hyperlink ref="E4" r:id="rId25" xr:uid="{31541EE7-B42D-423E-9AA8-C216DE6B64A7}"/>
+    <hyperlink ref="F4" r:id="rId26" xr:uid="{395A83D0-9F08-4D83-854F-0AE6F1F29CBC}"/>
+    <hyperlink ref="F3" r:id="rId27" xr:uid="{58F9AB1E-5488-40A2-9983-26F11E828595}"/>
+    <hyperlink ref="E3" r:id="rId28" xr:uid="{5A8C1A72-92CF-4171-B7B9-E0254CBDE43F}"/>
+    <hyperlink ref="E24" r:id="rId29" xr:uid="{1F2E3E11-4862-43A4-AE5B-A25971038030}"/>
+    <hyperlink ref="F24" r:id="rId30" xr:uid="{82182BB5-27E4-45A0-9245-90B695825443}"/>
+    <hyperlink ref="E9" r:id="rId31" xr:uid="{06ECC9D7-A685-4D13-AE11-5DD9C258A7EE}"/>
+    <hyperlink ref="J5" r:id="rId32" xr:uid="{BEC89C47-1D25-4DE9-AC71-083FAD0B34C3}"/>
+    <hyperlink ref="E20" r:id="rId33" xr:uid="{3FA1CD4F-2381-4BF1-8F3E-F2B2EC7ACF85}"/>
+    <hyperlink ref="E32" r:id="rId34" xr:uid="{6143B28D-A231-422C-9F6E-9D22A5EE20EC}"/>
+    <hyperlink ref="F34" r:id="rId35" xr:uid="{F50C1EB9-5D1C-4B95-B429-377D59A03513}"/>
+    <hyperlink ref="E34" r:id="rId36" xr:uid="{215E8F44-72B5-4AED-B8B7-3F716C2C9FED}"/>
+    <hyperlink ref="E22" r:id="rId37" xr:uid="{00990BE2-D559-46EF-86D1-57D51622C40D}"/>
+    <hyperlink ref="F22" r:id="rId38" xr:uid="{DCD02053-CEBB-4E57-904F-A030DF9C21A9}"/>
+    <hyperlink ref="E12" r:id="rId39" xr:uid="{AEC3391B-7D1E-4D91-B2D0-7C05910F189D}"/>
+    <hyperlink ref="F12" r:id="rId40" xr:uid="{DFC08211-F9CC-4B7C-BE88-90F525577256}"/>
+    <hyperlink ref="F21" r:id="rId41" xr:uid="{DA238934-A9D6-41DF-A7D3-02C52609E7A4}"/>
+    <hyperlink ref="E21" r:id="rId42" xr:uid="{BE1025E4-0C8B-464A-94DB-E1029F52499B}"/>
+    <hyperlink ref="F39" r:id="rId43" xr:uid="{A667CFB0-7B94-472E-9628-6E081DEF139A}"/>
+    <hyperlink ref="E39" r:id="rId44" xr:uid="{1C4AFCD6-DEF8-42D4-A41B-2335EDE91552}"/>
+    <hyperlink ref="F36" r:id="rId45" xr:uid="{6A71B6A8-01BB-4EC2-A1E1-3A9FC5E427FC}"/>
+    <hyperlink ref="E36" r:id="rId46" xr:uid="{A60CB216-EF26-4335-B9A8-9667A0871FCE}"/>
+    <hyperlink ref="F13" r:id="rId47" xr:uid="{BF2B90AA-CB55-4147-84AC-0500086745BF}"/>
+    <hyperlink ref="E13" r:id="rId48" xr:uid="{5A9C1536-19AB-4B66-A33C-E94FAEA8DC33}"/>
+    <hyperlink ref="E26" r:id="rId49" xr:uid="{6B3F056B-BE9E-410D-A402-D0B7A082F8FF}"/>
+    <hyperlink ref="F26" r:id="rId50" xr:uid="{5FFF6BB5-6911-47ED-A878-31F14AA4CCB6}"/>
+    <hyperlink ref="F7" r:id="rId51" xr:uid="{9567CA2D-EFE1-41F8-948A-768765025D60}"/>
+    <hyperlink ref="E7" r:id="rId52" xr:uid="{A1309773-A5F2-461B-9FD5-6F306A4FD457}"/>
+    <hyperlink ref="E29" r:id="rId53" xr:uid="{A162F40D-F6FD-4099-A350-D0002A3057DA}"/>
+    <hyperlink ref="F29" r:id="rId54" xr:uid="{E01788B1-A80B-48E9-9E16-744B2433ED75}"/>
+    <hyperlink ref="F25" r:id="rId55" xr:uid="{779B7301-2CC3-4C4F-8FC3-C6FD68C1B77A}"/>
+    <hyperlink ref="E25" r:id="rId56" xr:uid="{AFCDF617-1F40-451D-88A8-8E755B3BE1D2}"/>
+    <hyperlink ref="E35" r:id="rId57" xr:uid="{FC1DB418-6772-4F8C-82D8-5AF5628D3AC3}"/>
+    <hyperlink ref="F14" r:id="rId58" xr:uid="{16C94B7E-E6C6-4CF0-B928-AD2B73500472}"/>
+    <hyperlink ref="F35" r:id="rId59" location="citeas" xr:uid="{D1B3B81C-2F82-4629-9FC1-4353AB605B76}"/>
+    <hyperlink ref="E14" r:id="rId60" xr:uid="{656876C3-5D28-4ECE-B160-137885BBD472}"/>
+    <hyperlink ref="F17" r:id="rId61" xr:uid="{1CDD0BF3-93DF-4629-8D83-4C995F3FBAEA}"/>
+    <hyperlink ref="E17" r:id="rId62" xr:uid="{1E99DCCD-93C8-47BD-AB1B-F096AD30B672}"/>
+    <hyperlink ref="F19" r:id="rId63" xr:uid="{BA058841-70A9-4578-BDA8-2B610D7F798E}"/>
+    <hyperlink ref="E19" r:id="rId64" xr:uid="{E7A0EF1E-D431-4572-B9D4-313436BB39A8}"/>
+    <hyperlink ref="F18" r:id="rId65" xr:uid="{B110DB8E-16E9-47DF-90DB-9713B248B748}"/>
+    <hyperlink ref="F23" r:id="rId66" xr:uid="{BE0E25E4-720D-43DC-BA86-AC4CAAF9C963}"/>
+    <hyperlink ref="E23" r:id="rId67" xr:uid="{8B9D759F-81A0-4BAB-A68F-F8FAA98330AE}"/>
+    <hyperlink ref="F27" r:id="rId68" xr:uid="{BD2F2414-265C-4ECF-9E09-71CC6602CB5C}"/>
+    <hyperlink ref="E27" r:id="rId69" xr:uid="{FCD02C76-FDEC-49EE-80EF-34CED8D9D6B6}"/>
+    <hyperlink ref="E15" r:id="rId70" xr:uid="{584D0A85-BBC0-4358-BB54-87D73785496D}"/>
+    <hyperlink ref="F11" r:id="rId71" xr:uid="{27264864-EE95-448C-811F-BA85099EF2D9}"/>
+    <hyperlink ref="E11" r:id="rId72" xr:uid="{EEF03948-E49B-486E-817D-EEE788F4CEAE}"/>
+    <hyperlink ref="F10" r:id="rId73" xr:uid="{DE92A6AE-A2E4-46C7-8FFF-C5F1A12E2ACB}"/>
+    <hyperlink ref="E10" r:id="rId74" xr:uid="{F96F71DF-0664-4DD1-88E4-CBDF6565534B}"/>
+    <hyperlink ref="F6" r:id="rId75" xr:uid="{86D7A23D-5E99-4CD5-B311-DD9D8A173C8C}"/>
+    <hyperlink ref="E6" r:id="rId76" xr:uid="{30A4C8C1-66D0-4C23-8217-B4C3DB83F2EA}"/>
+    <hyperlink ref="F8" r:id="rId77" xr:uid="{E4965881-1403-4F79-8959-22D0A974E759}"/>
+    <hyperlink ref="E8" r:id="rId78" xr:uid="{1ACDBBF2-07D0-4487-B5C6-AC33BDA7AF67}"/>
+    <hyperlink ref="E37" r:id="rId79" xr:uid="{E8E131B3-579B-4EFE-A83D-5A610DE10758}"/>
+    <hyperlink ref="F38" r:id="rId80" xr:uid="{9DC437E2-9294-47A2-BC5D-A151DF6FF776}"/>
+    <hyperlink ref="E38" r:id="rId81" xr:uid="{2AB4D467-774B-410E-9786-1B3036659AD0}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId82"/>
@@ -3254,22 +3262,22 @@
   <sheetData>
     <row r="1" spans="1:6" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A1" s="27" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B1" s="33" t="s">
+        <v>67</v>
+      </c>
+      <c r="C1" s="27" t="s">
         <v>68</v>
       </c>
-      <c r="C1" s="27" t="s">
+      <c r="D1" s="27" t="s">
         <v>69</v>
       </c>
-      <c r="D1" s="27" t="s">
+      <c r="E1" s="27" t="s">
         <v>70</v>
       </c>
-      <c r="E1" s="27" t="s">
+      <c r="F1" s="27" t="s">
         <v>71</v>
-      </c>
-      <c r="F1" s="27" t="s">
-        <v>72</v>
       </c>
     </row>
     <row r="2" spans="1:6" ht="24" customHeight="1" x14ac:dyDescent="0.25">
@@ -3277,19 +3285,19 @@
         <v>1</v>
       </c>
       <c r="B2" s="30" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C2" s="29" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="D2" s="29" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="E2" s="29" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="F2" s="29" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="3" spans="1:6" ht="36" customHeight="1" x14ac:dyDescent="0.25">
@@ -3297,19 +3305,19 @@
         <v>2</v>
       </c>
       <c r="B3" s="30" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C3" s="35" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="D3" s="29" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="E3" s="29" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="F3" s="29" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="4" spans="1:6" ht="36" customHeight="1" x14ac:dyDescent="0.25">
@@ -3317,19 +3325,19 @@
         <v>3</v>
       </c>
       <c r="B4" s="30" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C4" s="35" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="D4" s="29" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="E4" s="29" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="F4" s="29" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="5" spans="1:6" ht="36" customHeight="1" x14ac:dyDescent="0.25">
@@ -3337,19 +3345,19 @@
         <v>4</v>
       </c>
       <c r="B5" s="30" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C5" s="35" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="D5" s="29" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="E5" s="29" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="F5" s="29" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="6" spans="1:6" ht="24" customHeight="1" x14ac:dyDescent="0.25">
@@ -3357,19 +3365,19 @@
         <v>5</v>
       </c>
       <c r="B6" s="30" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C6" s="35" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="D6" s="29" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="E6" s="29" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="F6" s="29" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="7" spans="1:6" ht="36" customHeight="1" x14ac:dyDescent="0.25">
@@ -3377,19 +3385,19 @@
         <v>6</v>
       </c>
       <c r="B7" s="30" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C7" s="35" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="D7" s="29" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="E7" s="29" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="F7" s="29" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="8" spans="1:6" ht="48" customHeight="1" x14ac:dyDescent="0.25">
@@ -3397,19 +3405,19 @@
         <v>7</v>
       </c>
       <c r="B8" s="30" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C8" s="35" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="D8" s="29" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="E8" s="29" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="F8" s="29" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="9" spans="1:6" ht="24" customHeight="1" x14ac:dyDescent="0.25">
@@ -3417,19 +3425,19 @@
         <v>8</v>
       </c>
       <c r="B9" s="30" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C9" s="29" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="D9" s="29" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="E9" s="29" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="F9" s="29" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="10" spans="1:6" ht="36" customHeight="1" x14ac:dyDescent="0.25">
@@ -3437,19 +3445,19 @@
         <v>9</v>
       </c>
       <c r="B10" s="34" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C10" s="36" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="D10" s="32" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="E10" s="32" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="F10" s="32" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
   </sheetData>
@@ -3469,15 +3477,15 @@
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B1" s="61" t="s">
-        <v>53</v>
-      </c>
-      <c r="C1" s="61"/>
-      <c r="D1" s="61"/>
-      <c r="E1" s="61"/>
-      <c r="F1" s="61"/>
-      <c r="G1" s="61"/>
-      <c r="H1" s="61"/>
+      <c r="B1" s="63" t="s">
+        <v>52</v>
+      </c>
+      <c r="C1" s="63"/>
+      <c r="D1" s="63"/>
+      <c r="E1" s="63"/>
+      <c r="F1" s="63"/>
+      <c r="G1" s="63"/>
+      <c r="H1" s="63"/>
     </row>
     <row r="2" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B2" t="s">

</xml_diff>